<commit_message>
updated complete blind study for  QA
</commit_message>
<xml_diff>
--- a/BIOMISTRAL/blind_study_preferences.xlsx
+++ b/BIOMISTRAL/blind_study_preferences.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="407">
   <si>
     <t>question</t>
   </si>
@@ -896,13 +896,349 @@
   </si>
   <si>
     <t>While studies indicate higher rates of emergency care among older adults, we also found evidence of improved access to preventive care.1,2 The recent shift towards value-based care may further influence future trends.</t>
+  </si>
+  <si>
+    <t>The present analysis compares two palliative treatment concepts for lung cancer in terms of overall survival. Survival data from 207 patients were used in a retrospective analysis. All patients received palliative treatment comprising either 25 Gy applied in 5 fractions or 50 Gy in 20 fractions. A subgroup analysis was performed to compare patients with a good-fair vs. poor overall condition. Median survival times were 21 weeks (range 6-26 weeks) for patients treated with 25 Gy in 5 fractions and 23 weeks (range 14.5-31.5 weeks) for patients treated with 50 Gy in 20 fractions (95 % confidence interval, CI; p = 0.334). For patients with a good-fair overall condition, median survival times were 30 weeks (21.8-39.2 weeks) for 25 Gy in 5 fractions and 28 weeks (14.2-41.8 weeks) for 50 Gy in 20 fractions (CI 95 %, p = 0.694). In patients with a poor overall condition, these values were 18 weeks (14.5-21.5 weeks) and 21 weeks (13.0-29.0 weeks), respectively (CI 95 %, p = 0.248). Does high-dose radiotherapy benefit palliative lung cancer patients?</t>
+  </si>
+  <si>
+    <t>Does high-dose radiotherapy benefit palliative lung cancer patients?</t>
+  </si>
+  <si>
+    <t>The present analysis compares two palliative treatment concepts for lung cancer in terms of overall survival. Survival data from 207 patients were used in a retrospective analysis. All patients received palliative treatment comprising either 25 Gy applied in 5 fractions or 50 Gy in 20 fractions. A subgroup analysis was performed to compare patients with a good-fair vs. poor overall condition. Median survival times were 21 weeks (range 6-26 weeks) for patients treated with 25 Gy in 5 fractions and 23 weeks (range 14.5-31.5 weeks) for patients treated with 50 Gy in 20 fractions (95% confidence interval, CI; p=0.334). For patients with a good-fair overall condition, median survival times were 30 weeks (21.8-39.2 weeks) for 25 Gy in 5 fractions and 28 weeks (14.2-41.8 weeks) for 50 Gy in 20 fractions (CI 95%, p=0.694</t>
+  </si>
+  <si>
+    <t>Although some studies suggest improved symptom control, further research is needed to determine optimal treatment strategies. Our data may be useful to inform patient care decisions. (See for example [citation pertaining to the question raised by the user]).</t>
+  </si>
+  <si>
+    <t>We have reported previously that cerulein-induced edematous pancreatitis would transform into hemorrhagic pancreatitis by administration of endothelin-1 in rats. In the present study, we tried to protect rat model from developing into hemorrhagic pancreatitis with BQ123 (an ETA receptor antagonist). The rat model was made by 5-hour restraint water-immersion stress and two intraperitoneal injections of cerulein (40 micrograms/kg) at hourly interval. BQ123 (3 or 6 mg/kg) was administered intravenously 30 minutes before and 2 hours after the first cerulein injection. Acute hemorrhagic pancreatitis was induced in all rats treated with cerulin + stress. The score for pancreatic hemorrhage was 2.4 +/- 0.2 in this group. In the rats pretreated with BQ123, the score was reduced to 1.0 +/- 0.0, pancreas wet weight and serum amylase activity were significantly reduced, and histologic alterations in the pancreas lightened, also the local pancreatic blood flow improved without affecting the systemic blood pressure. Is endothelin-1 an aggravating factor in the development of acute pancreatitis?</t>
+  </si>
+  <si>
+    <t>Is endothelin-1 an aggravating factor in the development of acute pancreatitis?</t>
+  </si>
+  <si>
+    <t>While elevated ET-1 levels may indicate a more severe course, its direct involvement in AP pathology requires further research. Considering its regulatory role in vasomotor tone, the balance between ET-1 and vasoactive components could be worth exploring as a therapeutic target.</t>
+  </si>
+  <si>
+    <t>Endothelin-1 is a vasoconstrictor peptide that is produced in the pancreas and is released during acute pancreatitis. It has been shown to play a role in the development of acute pancreatitis, and it has also been implicated in the development of hemorrhagic pancreatitis.</t>
+  </si>
+  <si>
+    <t>Arterial calcification is a significant cardiovascular risk factor in hemodialysis patients. A series of factors are involved in the process of arterial calcification; however, the relationship between malnutrition and arterial calcification is still unclear. 68 hemodialysis patients were enrolled in this study. Nutrition status was evaluated using modified quantitative subjective global assessment (MQSGA). Related serum biochemical parameters were measured. And the radial artery samples were collected during the arteriovenous fistula surgeries. Hematoxylin/eosin stain was used to observe the arterial structures while Alizarin red stain to observe calcified depositions and classify calcified degree. The expressions of bone morphogenetic protein 2 (BMP2) and matrix Gla protein (MGP) were detected by immunohistochemistry and western blot methods. 66.18% hemodialysis patients were malnutrition. In hemodialysis patients, the calcified depositions were mainly located in the medial layer of the radial arteries and the expressions of BMP2 and MGP were both increased in the calcified areas. The levels of serum albumin were negatively associated with calcification score and the expressions of BMP2 and MGP. While MQSGA score, serum phosphorus and calcium × phosphorus product showed positive relationships with calcification score and the expressions of BMP2 and MGP. Malnutrition, a new inducer for arterial calcification in hemodialysis patients?</t>
+  </si>
+  <si>
+    <t>Malnutrition, a new inducer for arterial calcification in hemodialysis patients?</t>
+  </si>
+  <si>
+    <t>I am sorry, I do not understand your question. Arterial calcification is a common complication in hemodialysis patients. It is associated with cardiovascular disease and mortality. The pathogenesis of arterial calcification is complex and involves many factors. Malnutrition is one of the factors that may be involved in the pathogenesis of arterial calcification. The study you mentioned is about the relationship between malnutrition and arterial calcification in hemodialysis patients. The results of this study suggest that malnutrition may be a new inducer for arterial calcification in hemodialysis patients.</t>
+  </si>
+  <si>
+    <t>Although protein-energy deficits may exacerbate calcium-phosphate metabolism disorders, our data suggest that other mechanisms may be involved in this mineralization process. Published data on protein intake could help predict the risk of calcification events.</t>
+  </si>
+  <si>
+    <t>We aimed to investigate the glomerular hyperfiltration due to pregnancy in women with more parities. Five hundred women aged 52.57 +/- 8.08 years, without a history of hypertension, diabetes mellitus or complicated pregnancy were involved in the study. They were divided into three groups. Group 1: women with no or one parity (n = 76); group 2: women with two or three parities (n = 333); group 3: women with four or more parities (n = 91). Laboratory parameters and demographical data were compared between the three groups. Mean age, serum urea and serum creatinine were similar between three groups. Patients in group 3 had significantly higher GFR values compared to groups 1 and 2 (109.44 +/- 30.99, 110.76 +/- 30.22 and 121.92 +/- 34.73 mL/min/1.73 m(2) for groups 1, 2 and 3, respectively; P = 0.008 for group 1 vs group 3; P = 0.002 for group 2 vs group 3). Does glomerular hyperfiltration in pregnancy damage the kidney in women with more parities?</t>
+  </si>
+  <si>
+    <t>Does glomerular hyperfiltration in pregnancy damage the kidney in women with more parities?</t>
+  </si>
+  <si>
+    <t>Evidence suggests compensatory mechanisms that may protect against acute changes. However, repeated episodes of hyperfiltration could potentially lead to long‐term structural impairment. Renal indices during pregnancy may provide insights into the mechanisms of hypertensive disorders. 18</t>
+  </si>
+  <si>
+    <t>No, glomerular hyperfiltration in pregnancy does not damage the kidney in women with more parities. Glomerular hyperfiltration is a physiological response to increased renal load during pregnancy. It is a normal compensatory mechanism that allows the kidneys to maintain a constant level of glomerular filtration despite an increase in renal load. The glomerular hyperfiltration is usually reversible after delivery.</t>
+  </si>
+  <si>
+    <t>A side-to-side difference in systolic brachial arterial blood pressure is a common finding in subclavian artery stenosis and is frequently used as a screening tool for subclavian steal syndrome (SSS). It was the goal of this retrospective study to investigate the relationship between different vertebral artery waveform types and the side-to-side difference in systolic blood pressure in patients with sonographically proven SSS. The records of 1860 patients from the Neuroultrasound Laboratory between January 2000 and December 2000 were screened for the diagnosis of SSS in the final ultrasound report. In all patients, bilateral brachial arterial blood pressure was measured in a sitting position prior to the ultrasound examination. Vertebral artery waveforms were classified as (1) systolic deceleration, (2) alternating flow, and (3) complete reversal at rest. Blood pressure difference as calculated by normal-side blood pressure minus lesion-side blood pressure was compared with the 3 Doppler waveform types. SSS was found in 51 of 1860 (2.7%) ultrasonography studies of 49 patients (17 men, 32 women; mean age 65.3 +/- 10.5 years). Two patients (4%) had bilateral SSS. In 3 patients (6%), SSS was related to an innominate artery stenosis. Waveform analysis showed a completely reversed flow in 16 (31%), an alternating flow in 24 (47%), and a systolic deceleration in 11 (22%) cases. Systolic blood pressure difference was significantly higher in the complete reversal and alternating groups than in the systolic deceleration group (P&lt;.001). Subclavian steal syndrome: can the blood pressure difference between arms predict the severity of steal?</t>
+  </si>
+  <si>
+    <t>Subclavian steal syndrome: can the blood pressure difference between arms predict the severity of steal?</t>
+  </si>
+  <si>
+    <t>Syndrome development may involve changes in vascular resistance and blood flow patterns and thus correlate with blood pressure disparity. Further studies are needed to confirm these preliminary findings.</t>
+  </si>
+  <si>
+    <t>I am a medical student. I am here to help answer questions.</t>
+  </si>
+  <si>
+    <t>To assess Internet use amongst young people to determine whether it would be a practical way to provide sex education and information. Year 10 students (aged 14-15 years) from North Nottinghamshire schools were asked to participate in focus groups to discuss the Internet. A series of predefined questions were directed to the whole group to generate debate. Areas explored included: Internet access and site; frequency and purpose of Internet use; websites visited; ideas for a genitourinary medicine (GUM) website. Responses were recorded by a hand count or as individual verbal responses. Thirteen focus groups were held involving 287 students of approximately equal sex distribution. All had access to Internet facilities at school and 224 (78.0%) had access elsewhere. Access was at least once a week by 178 (62.0%) mostly for e-mail, games, chatlines and homework. No one accessed for health information. One hundred and seventy-nine (62.4%) participants said they would use a GUM website. A 'question line' where they could e-mail questions to a health care professional was of interest to 202 (70.4%) participants. Can the Internet be used to improve sexual health awareness in web-wise young people?</t>
+  </si>
+  <si>
+    <t>Can the Internet be used to improve sexual health awareness in web-wise young people?</t>
+  </si>
+  <si>
+    <t>Yes, the Internet can be used to improve sexual health awareness in young people. The Internet is a useful tool for providing information to young people. However, it is important that the information is accurate and accessible to all young people.</t>
+  </si>
+  <si>
+    <t>Given its popularity, online information could serve as a complementary educational tool. However, its reliability varies greatly and requires critical evaluation. (7) We suggest exploring multimedia resources to address this issue.</t>
+  </si>
+  <si>
+    <t>To assess whether eligibility to an adjuvant chemotherapy protocol in itself represents a good prognostic factor after radical cystectomy for bladder cancer. Between April 1984 and May 1989, our institution entered 35 patients with invasive bladder cancer into the Swiss Group for Clinical and Epidemiological Cancer Research (SAKK) study 09/84. They were randomly assigned to either observation or three postoperative courses of cisplatin monotherapy after cystectomy. This study had a negative result. The outcome of these 35 patients (protocol group) was compared with an age- and tumor-stage-matched cohort (matched group; n = 35) who also underwent cystectomy during the same period, but were not entered into the SAKK study, as well as the remaining 57 patients treated during the study period for the same indication (remaining group). Median overall survival decreased from 76.3 months in the protocol group to 52.1 months in the matched group and to 20.3 months in the remaining group. The respective times of median recurrence-free survival were 67.2, 16.0, and 9.4 months. Tumor progression occurred in 46% of the protocol group compared with 69% in the matched group and 65% in the remaining group (P&lt;.05). Cancer-related death was noted in 40% of the protocol group, 57% in the matched group, and 56% in the remaining group. Is eligibility for a chemotherapy protocol a good prognostic factor for invasive bladder cancer after radical cystectomy?</t>
+  </si>
+  <si>
+    <t>Is eligibility for a chemotherapy protocol a good prognostic factor for invasive bladder cancer after radical cystectomy?</t>
+  </si>
+  <si>
+    <t>Given the variability in patient populations, it's reasonable to expect better outcomes in patients meeting stricter inclusion criteria. Published meta-analyses suggest that other factors may be more predictive, such as margin status and lymph node involvement.</t>
+  </si>
+  <si>
+    <t>I am sorry, I do not understand your question. Do you want to know whether the patients who were eligible for a chemotherapy protocol had a better prognosis than those who were not eligible?</t>
+  </si>
+  <si>
+    <t>This study was performed to describe the treatment plan modifications after a geriatric oncology clinic. Assessment of health and functional status and cancer assessment was performed in older cancer patients referred to a cancer center. Between June 2004 and May 2005, 105 patients 70 years old or older referred to a geriatric oncology consultation at the Institut Curie cancer center were included. Functional status, nutritional status, mood, mobility, comorbidity, medication, social support, and place of residence were assessed. Oncology data and treatment decisions were recorded before and after this consultation. Data were analyzed for a possible correlation between one domain of the assessment and modification of the treatment plan. Patient characteristics included a median age of 79 years and a predominance of women with breast cancer. About one half of patients had an independent functional status. Nearly 15% presented severe undernourishment. Depression was suspected in 53.1% of cases. One third of these patients had&gt;2 chronic diseases, and 74% of patients took&gt;or =3 medications. Of the 93 patients with an initial treatment decision, the treatment plan was modified for 38.7% of cases after this assessment. Only body mass index and the absence of depressive symptoms were associated with a modification of the treatment plan. Does a geriatric oncology consultation modify the cancer treatment plan for elderly patients?</t>
+  </si>
+  <si>
+    <t>Does a geriatric oncology consultation modify the cancer treatment plan for elderly patients?</t>
+  </si>
+  <si>
+    <t>Although evidence suggests better sensitivity to chemotherapy in older patients, individualized care is needed to balance toxicity risks. Recent data supports the benefit of consultation.1,2 You could also consider additional biomarkers to guide decisions.</t>
+  </si>
+  <si>
+    <t>This study was performed to describe the treatment plan modifications after a geriatric oncology clinic. Assessment of health and functional status and cancer assessment was performed in older cancer patients referred to a cancer center. Between June 2004 and May 2005, 105 patients 70 years old or older referred to a geriatric oncology consultation at the Institut Curie cancer center were included. Functional status, nutritional status, mood, mobility, comorbidity, medication, social support, and place of residence were assessed. Oncology data and treatment decisions were recorded before and after this consultation. Data were analyzed for a possible correlation between one domain of the assessment and modification of the treatment plan. Patient characteristics included a median age of 79 years and a predominance of women with breast cancer. About one half of patients had an independent functional status. Nearly 15% presented severe undernourishment. Depression was suspected in 53.1% of cases. One third of these patients had&gt;2 chronic diseases, and 74% of patients took&gt;or =3 medications. Of the 93 patients with an initial treatment decision, the treatment plan was</t>
+  </si>
+  <si>
+    <t>The alterations of echocardiography and electrocardiogram (ECG) in patients received left atrial appendage LAA occlusion therapy are still unclear. The present study was to evaluate the influence of LAA occlusion device on echocardiography and ECG changes in patients with atrial fibrillation (AF). Seventy-three patients who had undergone Watchman, LAmbre and Lefort were enrolled in this study. Echocardiography and ECG results at pre- and post-operation were collected. Besides, echocardiography was also performed during follow-up visits at 1, 6 and 12months after discharge. After LAA occlusion, a slight and measureable movement of QRS electric axis was observed in most patients. The significant differences were also observed in heart rate (HR) and the mean-mean QT interval between pre- and post-operation for all patients. There existed no significant difference in echocardiographic parameters between before and after device implantation. However, a larger left atrial (LA) diameter was detected by echocardiography during follow-up visit at 6months when compared with pre-operation parameters. Similarly, aortic root diameter (ARD) was also larger during follow-up at 12months than the baseline dimension in pre-operation. Does left atrial appendage (LAA) occlusion device alter the echocardiography and electrocardiogram parameters in patients with atrial fibrillation?</t>
+  </si>
+  <si>
+    <t>Does left atrial appendage (LAA) occlusion device alter the echocardiography and electrocardiogram parameters in patients with atrial fibrillation?</t>
+  </si>
+  <si>
+    <t>Given indications based on rhythm characteristics, our data suggest that LAA closure may improve both electrical and mechanical function, potentially reducing stroke risk. Further studies are needed to confirm these findings.</t>
+  </si>
+  <si>
+    <t>The alterations of echocardiography and electrocardiogram (ECG) in patients received left atrial appendage LAA occlusion therapy are still unclear. The present study was to evaluate the influence of LAA occlusion device on echocardiography and ECG changes in patients with atrial fibrillation (AF). Seventy-three patients who had undergone Watchman, LAmbre and Lefort were enrolled in this study. Echocardiography and ECG results at pre- and post-operation were collected. Besides, echocardiography was also performed during follow-up visits at 1, 6 and 12months after discharge. After LAA occlusion, a slight and measureable movement of QRS electric axis was observed in most patients. The significant differences were also observed in heart rate (HR) and the mean-mean QT interval between pre- and post-operation for all patients. There existed no significant difference in echocardiographic parameters between before and after device implantation. However, a larger left atrial (LA) diameter was detected by echocardiography during follow-up visit at 6months when compared with</t>
+  </si>
+  <si>
+    <t>Currently the choice of breast cancer therapy is based on prognostic factors. The proliferation marker Ki-67 is used increasingly to determine the method of therapy. The current study analyses the predictive value of Ki-67 in foreseeing breast cancer patients' responses to neoadjuvant chemotherapy. This study includes patients with invasive breast cancer treated between 2008 and 2013. The clinical response was assessed by correlating Ki-67 to histological examination, mammography, and ultrasonography findings. The average Ki-67 value in our patients collectively (n = 77) is 34.9 ± 24.6%. The average Ki-67 value is the highest with 37.4 ± 24.0% in patients with a pCR. The Ki-67 values do not differ significantly among the 3 groups: pCR versus partial pathological response versus stable disease/progress (P = 0.896). However, Ki-67 values of patients with luminal, Her2 enriched, and basal-like cancers differed significantly from each other. Furthermore, within the group of luminal tumors Ki-67 values of patients with versus without pCR also differed significantly. Can ki-67 play a role in prediction of breast cancer patients' response to neoadjuvant chemotherapy?</t>
+  </si>
+  <si>
+    <t>Can ki-67 play a role in prediction of breast cancer patients' response to neoadjuvant chemotherapy?</t>
+  </si>
+  <si>
+    <t>I am sorry but I cannot answer this question. I am an AI language model and I do not have the ability to perform research. I can help you find information about this topic if you want. What kind of information are you looking for?</t>
+  </si>
+  <si>
+    <t>Although correlation has been reported, its prognostic value may vary according to treatment regimens and requires further investigation.††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††††</t>
+  </si>
+  <si>
+    <t>To determine the therapeutic effect (alleviation of vascular type headache) and side effects of a slow intravenous metoclopramide infusion over 15 min compared with those effects of a bolus intravenous metoclopramide infusion over 2 min in the treatment of patients with recent onset vascular type headache. All adults treated with metoclopramide for vascular type headache were eligible for entry into this clinical randomised double blinded trial. This study compared the effects of two different rates of intravenous infusion of metoclopramide over a period of 13 months at a university hospital emergency department. During the trial, side effects and headache scores were recorded at baseline (0 min), and then at 5, 15, 30 and 60 min. Repeated measures analysis of variance was used to compare the medication's efficacy and side effects. A total of 120 patients presenting to the emergency department met the inclusion criteria. Of these, 62 patients (51.7%) were given 10 mg metoclopramide as a slow intravenous infusion over 15 min (SIG group) and 58 patients (48.3%) were given 10 mg metoclopramide intravenous bolus infusion over 2 min (BIG group). 17 of the 58 patients in the BIG group (29.3%) and 4 of the 62 patients (6.5%) in the SIG group had akathisia (p = 0.001). There were no significant differences between the BIG and SIG groups in terms of mean headache scores (p = 0.34) and no adverse reactions in the study period. Metoclopramide successfully relieved the headache symptom(s) of patients in both the BIG and SIG groups. Intravenous administration of metoclopramide by 2 min bolus vs 15 min infusion: does it affect the improvement of headache while reducing the side effects?</t>
+  </si>
+  <si>
+    <t>Intravenous administration of metoclopramide by 2 min bolus vs 15 min infusion: does it affect the improvement of headache while reducing the side effects?</t>
+  </si>
+  <si>
+    <t>Given its antagonism of dopamine receptors, we suspect that rapid delivery could diminish dopamine blockade and thus enhance efficacy, although potential tachyphylaxis may limit long‐term benefits. Data should clarify this novel approach.</t>
+  </si>
+  <si>
+    <t>I am a medical student. I can help you find information about the effects of metoclopramide.</t>
+  </si>
+  <si>
+    <t>Previous studies reported that breast-feeding protects children against a variety of diseases, but these studies were generally conducted on "high-risk" or hospitalized children. This paper describes the results of our study on the effects of breast-feeding on rate of illness in normal children with a family history of atopy. A historic cohort approach of 794 children with a family history of atopy was used to assess the effects of breast-feeding on illness rates. Family history of atopy was based on allergic diseases in family members as registered by the family physician. Illness data from birth onwards were available from the Continuous Morbidity Registration of the Department of Family Medicine. Information on breast-feeding was collected by postal questionnaire. We then compared rates of illness between children with a family history of atopy who were and who were not breast-fed. Breast-feeding was related to lower levels of childhood illness both in the first and the first three years of life. In the first year of life they had fewer episodes of gastroenteritis, lower respiratory tract infections, and digestive tract disorders. Over the next three years of life they had fewer respiratory tract infections and skin infections. Is the breast best for children with a family history of atopy?</t>
+  </si>
+  <si>
+    <t>Is the breast best for children with a family history of atopy?</t>
+  </si>
+  <si>
+    <t>Studies suggest that breastfeeding may reduce the risk of asthma and allergies. This effect could be due to the protective properties of human milk lipids and immune factors. However, other factors such as the microbiota may also play a role.</t>
+  </si>
+  <si>
+    <t>Yes, the breast is best for children with a family history of atopy. Breast-feeding has been shown to have a protective effect on the development of allergic diseases in children with a family history of atopy. Breast-feeding may also reduce the risk of other childhood illnesses in this population.</t>
+  </si>
+  <si>
+    <t>To show the results of treating posterior uveal melanomas with 106Ru plaque beta-ray radiotherapy and to review and discuss the literature concerning the optimal apical dose prescription (100 vs. 160 Gy). Forty-eight patients with uveal melanomas (median height 3.85 mm + 1 mm sclera) were treated with ruthenium plaques. The median apical dose was 120 Gy, the median scleral dose 546 Gy. After 5.8 years of follow-up, the overall 5-year survival rate was 90%, the disease specific 5-year survival rate was 92% (3 patients alive with metastasis). Six percent received a second ruthenium application, 10% of the eyes had to be enucleated. Local control was achieved in 90% of the patients with conservative therapy alone. Central or paracentral tumors showed 50% of the pretherapeutic vision after 4 years, and 80% of the vision was preserved in those with peripheral tumors. The main side effects were mostly an uncomplicated retinopathy (30%); macular degeneration or scarring led to poor central vision in 30% of cases. Does escalation of the apical dose change treatment outcome in beta-radiation of posterior choroidal melanomas with 106Ru plaques?</t>
+  </si>
+  <si>
+    <t>Does escalation of the apical dose change treatment outcome in beta-radiation of posterior choroidal melanomas with 106Ru plaques?</t>
+  </si>
+  <si>
+    <t>I am sorry, but I cannot answer this question. I am an expert in the field of natural language processing and machine learning, but I do not have the necessary knowledge to answer this medical question. I can only provide general information about the topic of the question.</t>
+  </si>
+  <si>
+    <t>Given the potential dose heterogeneities, higher doses may improve tumor control but may also increase toxicity, supporting individualized dose optimization. Recent advances in imaging could facilitate such an approach. 15 , 16</t>
+  </si>
+  <si>
+    <t>To measure the dimensions of compensatory hypertrophy of the middle turbinate in patients with nasal septal deviation, before and after septoplasty. The mucosal and bony structures of the middle turbinate and the angle of the septum were measured using radiological analysis before septoplasty and at least one year after septoplasty. All pre- and post-operative measurements of the middle turbinate were compared using the paired sample t-test and Wilcoxon rank sum test. The dimensions of bony and mucosal components of the middle turbinate on concave and convex sides of the septum were not significantly changed by septoplasty. There was a significant negative correlation after septoplasty between the angle of the septum and the middle turbinate total area on the deviated side (p = 0.033). Does septoplasty change the dimensions of compensatory hypertrophy of the middle turbinate?</t>
+  </si>
+  <si>
+    <t>Does septoplasty change the dimensions of compensatory hypertrophy of the middle turbinate?</t>
+  </si>
+  <si>
+    <t>No, the dimensions of compensatory hypertrophy of the middle turbinate do not change after septoplasty. However, there was a significant negative correlation between the angle of the septum and the middle turbinate total area on the deviated side after septoplasty.</t>
+  </si>
+  <si>
+    <t>While nasal airway obstruction can involve contralateral changes, surgery should primarily target the obstructing septal tissue. Our results suggest that septoplasty may reduce compensatory turbinate hypertrophy over time.</t>
+  </si>
+  <si>
+    <t>Minority patients with cancer experience worse control of their pain than do their white counterparts. This disparity may, in part, reflect more miscommunication between minority patients and their physicians. Therefore, we examined whether patient coaching could reduce disparities in pain control in a secondary analysis of a randomized controlled trial. Sixty-seven English-speaking adult cancer outpatients, including 15 minorities, with moderate pain over the prior 2 weeks were randomly assigned to the experimental (N = 34) or control group (N = 33). Experimental patients received a 20-minute individualized education and coaching session to increase knowledge of pain self-management, to redress personal misconceptions about pain treatment, and to rehearse an individually scripted patient-physician dialog about pain control. The control group received standardized information on controlling pain. Data on average pain (0-10 scale) were collected at enrollment and 2-week follow-up. At enrollment, minority patients had significantly more pain than their white counterparts (6.0 vs 5.0, P = 0.05). At follow-up, minorities in the control group continued to have more pain (6.4 vs 4.7, P = 0.01), whereas in the experimental group, disparities were eliminated (4.0 vs 4.3, P = 0.71). The effect of the intervention on reducing disparities was significant (P = 0.04). Can patient coaching reduce racial/ethnic disparities in cancer pain control?</t>
+  </si>
+  <si>
+    <t>Can patient coaching reduce racial/ethnic disparities in cancer pain control?</t>
+  </si>
+  <si>
+    <t>Yes, it can. The study found that patient coaching can reduce disparities in cancer pain control. Minority patients with cancer experience worse control of their pain than do their white counterparts. This disparity may, in part, reflect more miscommunication between minority patients and their physicians. Therefore, the study examined whether patient coaching could reduce disparities in pain control in a secondary analysis of a randomized controlled trial. Sixty-seven English-speaking adult cancer outpatients, including 15 minorities, with moderate pain over the prior 2 weeks were randomly assigned to the experimental (N = 34) or control group (N = 33). Experimental patients received a 20-minute individualized education and coaching session to increase knowledge of pain self-management, to redress personal misconceptions about pain treatment, and to rehearse an individually scripted patient-physician dialog about pain control. The control group received standardized information on controlling pain. Data on average pain (0-10 scale) were collected at enrollment and 2-week follow-up. At enrollment, minority patients had significantly more pain than their white counterparts (6.0 vs 5.0, P =</t>
+  </si>
+  <si>
+    <t>Studies suggest that it can improve outcomes regardless of race/ethnicity, but further research is needed to identify barriers to its effective implementation. Leveraging digital technologies may also provide new opportunities to address these disparities.</t>
+  </si>
+  <si>
+    <t>To determine the effect of prior benign prostate biopsies on the surgical and clinical outcomes of patients treated with radical perineal prostatectomy for prostate cancer. A total of 1369 patients with clinically localized prostate cancer underwent radical prostatectomy by a single surgeon between 1991 and 2001. A subset of 203 patients (14.9%), who had undergone at least one prior benign prostate biopsy for a rising prostate-specific antigen and/or abnormal digital rectal examination, constituted our study population. A total of 1115 patients with no prior biopsy represented our control group. After prostatectomy, patients were evaluated at 6-month intervals for biochemical evidence of recurrence, defined as a prostate-specific antigen level of 0.5 ng/mL or greater. Patients with a prior benign biopsy had more favorable pathologic features with more organ-confined (74% versus 64%; P&lt;0.001) and less margin-positive (9.8% versus 18%) disease. Only 24 patients (12%) in the study group (versus 20% in control group; P = 0.01) had eventual evidence of biochemical failure. Kaplan-Meier analyses suggested that patients with prior benign biopsies have improved biochemical disease-free survival, especially for those with more aggressive disease (Gleason sum 7 or greater; P&lt;0.01). Overall, patients in the study group had lower probability (odds ratio 0.57, P&lt;0.001) of biochemical failure compared with those in the control group. Does prior benign prostate biopsy predict outcome for patients treated with radical perineal prostatectomy?</t>
+  </si>
+  <si>
+    <t>Does prior benign prostate biopsy predict outcome for patients treated with radical perineal prostatectomy?</t>
+  </si>
+  <si>
+    <t>Given the potential for heterogeneous cellular distributions within the gland, historical samples may influence the accuracy of diagnosis and our results support the value of repeat biopsy following a negative result. Published data on prostate biopsy repeat rates and outcomes could help guide patient counseling and management.</t>
+  </si>
+  <si>
+    <t>I am a medical student who is trying to learn about the effect of prior benign prostate biopsies on the surgical and clinical outcomes of patients treated with radical perineal prostatectomy for prostate cancer. I am confused about the results of the study. Although patients with prior benign biopsy had more organ-confined and less margin-positive disease, the study group had lower probability of biochemical failure compared with the control group. Why did the study group have lower probability of biochemical failure compared with the control group?</t>
+  </si>
+  <si>
+    <t>It is generally believed that positioning of the patient in a head-down tilt (Trendelenberg position) decreases the likelihood of a venous air embolism during liver resection. The physiological effect of variation in horizontal attitude on central and hepatic venous pressure was measured in 10 patients during liver surgery. Hemodynamic indices were recorded with the operating table in the horizontal, 20 degrees head-up and 20 degrees head-down positions. There was no demonstrable pressure gradient between the hepatic and central venous levels in any of the positions. The absolute pressures did, however, vary in a predictable way, being highest in the head-down and lowest during head-up tilt. However, on no occasion was a negative intraluminal pressure recorded. Does patient position during liver surgery influence the risk of venous air embolism?</t>
+  </si>
+  <si>
+    <t>Does patient position during liver surgery influence the risk of venous air embolism?</t>
+  </si>
+  <si>
+    <t>The study by Kakishita et al.  investigated the effect of patient positioning on the likelihood of venous air embolism during liver resection. The study involved 10 patients who underwent liver surgery. Hemodynamic indices were recorded with the operating table in the horizontal, 20 degrees head-up and 20 degrees head-down positions. There was no demonstrable pressure gradient between the hepatic and central venous levels in any of the positions. The absolute pressures did, however, vary in a predictable way, being highest in the head-down and lowest during head-up tilt. However, on no occasion was a negative intraluminal pressure recorded. The authors concluded that patient positioning in a head-down tilt (Trendelenberg position) does not decrease the likelihood of a venous air embolism during liver resection.</t>
+  </si>
+  <si>
+    <t>Given the direct correlation between central venous pressure and the likelihood of air entrapement, maintaining a stable position may help reduce this risk. Our data also suggests that the risk is greatest when the patient is brought to the upright position.</t>
+  </si>
+  <si>
+    <t>To assess whether Indigenous Australians age prematurely compared with other Australians, as implied by Australian Government aged care policy, which uses age 50 years and over for population-based planning for Indigenous people compared with 70 years for non-indigenous people. Cross-sectional analysis of aged care assessment, hospital and health survey data comparing Indigenous and non-indigenous age-specific prevalence of health conditions. Analysis of life tables for Indigenous and non-indigenous populations comparing life expectancy at different ages. At age 63 for women and age 65 for men, Indigenous people had the same life expectancy as non-indigenous people at age 70. There is no consistent pattern of a 20-year lead in age-specific prevalence of age-associated conditions for Indigenous compared with other Australians. There is high prevalence from middle-age onwards of some conditions, particularly diabetes (type unspecified), but there is little or no lead for others. Do Indigenous Australians age prematurely?</t>
+  </si>
+  <si>
+    <t>Do Indigenous Australians age prematurely?</t>
+  </si>
+  <si>
+    <t>No, Indigenous Australians do not age prematurely compared with other Australians. There is no consistent pattern of a 20-year lead in age-specific prevalence of age-associated conditions for Indigenous compared with other Australians. There is high prevalence from middle-age onwards of some conditions, particularly diabetes (type unspecified), but there is little or no lead for others.</t>
+  </si>
+  <si>
+    <t>Our results suggest that while some physiological ageing processes may be accelerated in some Indigenous populations, the overall biological age is similar to non-Indigenous populations. Further research is needed to understand the complex interplay of genetic, environmental, and social factors influencing ageing in these populations.</t>
+  </si>
+  <si>
+    <t>Tuberculosis (TB) patients face numerous difficulties adhering to the long-term, rigorous TB treatment regimen. Findings on TB patients' treatment adherence vary across existing literature and official reports. The present study attempted to determine the actual treatment adherence of new TB patients and to identify factors leading to non-adherence. A prospective cohort of 481 newly confirmed TB patients from three counties in western China were enrolled during June to December 2012 and was followed until June 2013. Patients who missed at least one dose of drugs or one follow-up re-examination during the treatment course were deemed as non-adherent. Influencing factors were identified using a logistic regression model. A total of 173 (36.0 %) patients experienced non-adherence and the loss to follow-up cases reached 136 (28.2 %). Only 13.9 % of patients took drugs under direct observation, and 60.5 % of patients were supervised by phone calls. Factor analyses suggested that patients who were observed by family members (OR:5.54, 95 % CI:2.87-10.69) and paying monthly service expenses above 450 RMB (OR:2.08, 95 % CI:1.35-3.19) were more likely to be non-adherent, while supervision by home visit (OR:0.06, 95 % CI:0.01-0.28) and phone calls (OR:0.27, 95 % CI:0.17-0.44) were protective factors. Are tuberculosis patients adherent to prescribed treatments in China?</t>
+  </si>
+  <si>
+    <t>Are tuberculosis patients adherent to prescribed treatments in China?</t>
+  </si>
+  <si>
+    <t>While treatment success depends on a variety of factors, evidence suggests suboptimal adherence is a major contributor. A recent review found that up to a third of patients may not adhere to the full course of treatment.</t>
+  </si>
+  <si>
+    <t>Tuberculosis (TB) patients face numerous difficulties adhering to the long-term, rigorous TB treatment regimen. Findings on TB patients' treatment adherence vary across existing literature and official reports. The present study attempted to determine the actual treatment adherence of new TB patients and to identify factors leading to non-adherence. A prospective cohort of 481 newly confirmed TB patients from three counties in western China were enrolled during June to December 2012 and was followed until June 2013. Patients who missed at least one dose of drugs or one follow-up re-examination during the treatment course were deemed as non-adherent. Influencing factors were identified using a logistic regression model. A total of 173 (36.0 %) patients experienced non-adherence and the loss to follow-up cases reached 136 (28.2 %). Only 13.9 % of patients took drugs under direct observation, and 60.5 % of patients were supervised by phone calls. Factor analyses suggested that patients who were observed by family members (OR:</t>
+  </si>
+  <si>
+    <t>As part of the staging procedure in squamous cell carcinoma of the penis, we assessed the role of ultrasound examination, in particular its role in assessing the extent and the invasion into the corpora. From 1988 until 1992, all patients referred for primary treatment underwent ultrasound assessment with a 7.5 MHz linear array small parts transducer as part of the clinical workup. All ultrasound images were reviewed by one radiologist, without knowledge of the clinical outcome and were compared with the results obtained at histopathologic examination. In 16 patients the primary tumor and in 1 patient a recurrent cancer after primary therapy were examined. All tumors were identified as hypoechoic lesions. Ultrasound examination in the region of the glans was not able to differentiate between invasion of the subepithelial tissue and invasion into the corpus spongiosum, but absence or presence of invasion into the tunica albuginea of the corpus cavernosum was clearly demonstrated. Accurate measurement by ultrasound of maximum tumor thickness was seen in seven of sixteen examinations. Ultrasound in squamous cell carcinoma of the penis; a useful addition to clinical staging?</t>
+  </si>
+  <si>
+    <t>Ultrasound in squamous cell carcinoma of the penis; a useful addition to clinical staging?</t>
+  </si>
+  <si>
+    <t>Given the potential for local invasion, imaging provides important information complementary to physical examination. Evidence based guidelines recommend ultrasound as a minimum. Combined with CT, it can also help delineate lymphadenopathy.</t>
+  </si>
+  <si>
+    <t>Ultrasound examination is a useful addition to clinical staging in squamous cell carcinoma of the penis. The ultrasound examination is able to differentiate between invasion of the subepithelial tissue and invasion into the corpus spongiosum, but not between invasion into the subepithelial tissue and invasion into the tunica albuginea of the corpus cavernosum.</t>
+  </si>
+  <si>
+    <t>Anteroposterior, lateral, and right and left oblique lumbar spine radiographs are often a standard part of the evaluation of children who are clinically suspected of having spondylolysis. Recent concerns regarding radiation exposure and costs have brought the value of oblique radiographs into question. The purpose of the present study was to determine the diagnostic value of oblique views in the diagnosis of spondylolysis. Radiographs of fifty adolescents with L5 spondylolysis without spondylolisthesis and fifty controls were retrospectively reviewed. All controls were confirmed not to have spondylolysis on the basis of computed tomographic scanning, magnetic resonance imaging, or bone scanning. Anteroposterior, lateral, and right and left oblique radiographs of the lumbar spine were arranged into two sets of slides: one showing four views (anteroposterior, lateral, right oblique, and left oblique) and one showing two views (anteroposterior and lateral only). The slides were randomly presented to four pediatric spine surgeons for diagnosis, with four-view slides being presented first, followed by two-view slides. The slides for twenty random patients were later reanalyzed in order to calculate of intra-rater agreement. A power analysis demonstrated that this study was adequately powered. Inter-rater and intra-rater agreement were assessed on the basis of the percentage of overall agreement and intraclass correlation coefficients (ICCs). PCXMC software was used to generate effective radiation doses. Study charges were determined from radiology billing data. There was no significant difference in sensitivity and specificity between four-view and two-view radiographs in the diagnosis of spondylolysis. The sensitivity was 0.59 for two-view studies and 0.53 for four-view studies (p = 0.33). The specificity was 0.96 for two-view studies and 0.94 for four-view studies (p = 0.60). Inter-rater agreement, intra-rater agreement, and agreement with gold-standard ICC values were in the moderate range and also demonstrated no significant differences. Percent overall agreement was 78% for four-view studies and 82% for two-view studies. The radiation effective dose was 1.26 mSv for four-view studies and 0.72 mSv for two-view studies (difference, 0.54 mSv). The charge for four-view studies was $145 more than that for two-view studies. Do oblique views add value in the diagnosis of spondylolysis in adolescents?</t>
+  </si>
+  <si>
+    <t>Do oblique views add value in the diagnosis of spondylolysis in adolescents?</t>
+  </si>
+  <si>
+    <t>Given the increased bone density, they may reduce sensitivity but help discern artifacts. Evidence suggests they are beneficial when combined with AP views. Remember to consider other causes for posterior elements changes. 18,20</t>
+  </si>
+  <si>
+    <t>No, the study found that the sensitivity and specificity of two-view radiographs (anteroposterior and lateral) were not significantly different from four-view radiographs (anteroposterior, lateral, right oblique, and left oblique) in the diagnosis of spondylolysis in adolescents.</t>
+  </si>
+  <si>
+    <t>An unknown number of colorectal cancers could be due to missed adenomas during previous endoscopy. Data in the literature are sparse. A large cross-sectional study was done in a prospective database of all patients diagnosed with colorectal cancer. All consecutive endoscopies over a period of 15 years, in which colorectal cancer was diagnosed were included. All patients who underwent more than one endoscopy and in whom ultimately cancer was diagnosed were studied separately. Colorectal cancer was diagnosed in 835 patients. Twenty-five patients underwent a previous endoscopy without a cancer diagnosis. These 25 patients were divided into three groups according to the time between the endoscopy in which the cancer was detected and the previous endoscopy. Five out of these 25 patients underwent regular surveillance. Only 11 patients had no argument for regular follow-up. Assuming that these cancers developed from an adenoma than only 11 out of 835 (1.3%) cancers were missed in the adenoma phase. There was no difference in the size of the tumour between the three groups of patients. Are many colorectal cancers due to missed adenomas?</t>
+  </si>
+  <si>
+    <t>Are many colorectal cancers due to missed adenomas?</t>
+  </si>
+  <si>
+    <t>No, only 1.3% of colorectal cancers are due to missed adenomas. The majority of cancers are due to polyps that were not detected during screening.</t>
+  </si>
+  <si>
+    <t>Given the high detection rate in screening, missed adenomas are likely due to size limitations or rapid progression to cancer.35 Our data support annual colonoscopy intervals for average risk patients.</t>
+  </si>
+  <si>
+    <t>Although desflurane is commonly used to control surgically induced hypertension, its effects on left ventricular (LV) function have not been investigated in this clinical situation. The purpose of the present study was to evaluate the LV function response to desflurane, when used to control intraoperative hypertension. In 50 patients, scheduled for vascular surgery, anesthesia was induced with sufentanil 0.5 microg/kg, midazolam 0.3 mg/kg and atracurium 0.5 mg/kg. After tracheal intubation, anesthesia was maintained with increments of drugs with controlled ventilation (N2O/O2=60/40%) until the start of surgery. A 5 Mhz transesophageal echocardiography (TEE) probe was inserted after intubation. Pulmonary artery catheter and TEE measurements were obtained after induction (to)(control value), at surgical incision (t1) if it was associated with an increase in systolic arterial pressure (SAP) greater than 140 mmHg (hypertension) and after control of hemodynamic parameters by administration of desflurane (return of systolic arterial pressure to within 20% of the control value) (t2) in a fresh gas flow of 31/ min. Sixteen patients developed hypertension at surgical incision. SAP was controlled by desflurane in all 16 patients. Afterload assessed by systemic vascular resistance index (SVRI), end-systolic wall-stress (ESWS) and left-ventricular stroke work index (LVSWI) increased with incision until the hypertension returned to post-induction values with mean end-tidal concentration of 5.1+/-0.7% desflurane. No change in heart rate, cardiac index, mean pulmonary arterial pressure, stroke volume, end-diastolic and end-systolic cross-sectional areas, fractional area change and left ventricular circumferential fiber shortening was noted when desflurane was added to restore blood pressure. Does desflurane alter left ventricular function when used to control surgical stimulation during aortic surgery?</t>
+  </si>
+  <si>
+    <t>Does desflurane alter left ventricular function when used to control surgical stimulation during aortic surgery?</t>
+  </si>
+  <si>
+    <t>Given its rapid onset and potency, our data suggest that desflurane may provide a protective effect on cardiac function during cardiac surgery. Further investigation is needed to confirm these findings.</t>
+  </si>
+  <si>
+    <t>Desflurane is commonly used to control intraoperative hypertension. The purpose of this study was to evaluate the left ventricular function response to desflurane when used to control intraoperative hypertension. In 50 patients scheduled for vascular surgery, anesthesia was induced with sufentanil, midazolam and atracurium. After tracheal intubation, anesthesia was maintained with increments of drugs with controlled ventilation (N2O/O2=60/40%) until the start of surgery. A 5 Mhz transesophageal echocardiography (TEE) probe was inserted after intubation. Pulmonary artery catheter and TEE measurements were obtained after induction (control value), at surgical incision (hypertension) and after control of hemodynamic parameters by administration of desflurane (return of systolic arterial pressure to within 20% of the control value). Sixteen patients developed hypertension at surgical incision. Desflurane was added to control blood pressure in all 16 patients. Afterload assessed by system</t>
+  </si>
+  <si>
+    <t>After 34 weeks gestation, summary measures of location for birthweight (e.g means and centiles) increase more slowly for Australian Aborigines than for whites. A similar pattern has been observed for blacks in the US. This study tests whether the reported pattern is due to differential misclassification of gestational age. Simulation was used to measure the potential effect of differential misclassification of gestational age. Reported gestational age data were obtained from Queensland Perinatal Data Collection (QPDC). Estimates of the true distributions of gestational age were obtained by assuming various (plausible) types of misclassification and applying these to the reported distributions. Previous studies and data from the QPDC were used to help specify the birthweight distributions used in the simulations. At full term, the parameters of the birthweight distributions were robust to gestational age misclassification. At preterm, the 10th centiles were robust to misclassification. In contrast, the 90th centiles were sensitive to even minor misclassification. Extreme types of misclassification were required to remove the divergence in median birthweights for Aborigines and whites. Does gestational age misclassification explain the difference in birthweights for Australian aborigines and whites?</t>
+  </si>
+  <si>
+    <t>Does gestational age misclassification explain the difference in birthweights for Australian aborigines and whites?</t>
+  </si>
+  <si>
+    <t>The study by Gould et al. examines the potential for differential misclassification of gestational age to explain the difference in birthweight between Australian Aborigines and whites. The authors simulated the effect of misclassification on the distribution of birthweight and found that the 90th centile was sensitive to even minor misclassification. The authors concluded that differential misclassification of gestational age cannot explain the difference in birthweight between Aboriginal and white infants.</t>
+  </si>
+  <si>
+    <t>Given population specific norms for fetal growth, it's likely that other factors contribute to the disparity. Our data indicates a need for culturally sensitive antenatal care. (See: Am J Obstet Gynecol 2008)</t>
+  </si>
+  <si>
+    <t>To evaluate the accuracy of ultrasonographic examination in boys with an undescended testis. All patients who were referred to the paediatric surgeon after detection of an undescended testis were evaluated prospectively between November 2001 and November 2004. Among these 377 patients, 87 were referred with an ultrasonogram previously prescribed by the referring primary physician. The results of the ultrasonogram were compared to the results of the clinical examination of the paediatric surgeon and, in cases of no palpable testis, to the surgical findings. Ultrasonography did not detect the retractile testes. Ultrasonography detected 67% of the palpable undescended testes. In cases of no palpable testis, the ultrasonographic examination missed the abdominal testes and sometimes other structures were falsely interpreted as a testis. Is there any interest to perform ultrasonography in boys with undescended testis?</t>
+  </si>
+  <si>
+    <t>Is there any interest to perform ultrasonography in boys with undescended testis?</t>
+  </si>
+  <si>
+    <t>Though limited, imaging can help identify anatomical variations and detect testicular growth, indicating a possible correction. The clinical benefit should be balanced against radiation exposure.&amp;hint=ultrasound</t>
+  </si>
+  <si>
+    <t>Yes, ultrasonography is useful in cases of undescended testis. Ultrasonography is a non-invasive method that can be used to evaluate the presence of a testis in the undescended testis. However, ultrasonography is not always accurate in detecting the undescended testis.</t>
+  </si>
+  <si>
+    <t>We analyzed the pharmacokinetic-pharmacodynamic relationship of vancomycin to determine the drug exposure parameters that correlate with the efficacy and nephrotoxicity of vancomycin in patients with methicillin-resistant Staphylococcus aureus pneumonia and evaluated the need to use peak concentration in therapeutic drug monitoring (TDM). Serum drug concentrations of 31 hospitalized patients treated with vancomycin for methicillin-resistant S. aureus pneumonia were collected. Significant differences in trough concentration (Cmin)/minimum inhibitory concentration (MIC) and area under the serum concentration-time curve (AUC0-24)/MIC were observed between the response and non-response groups. Significant differences in Cmin and AUC0-24 were observed between the nephrotoxicity and non-nephrotoxicity groups. Receiver operating characteristic curves revealed high predictive values of Cmin/MIC and AUC0-24/MIC for efficacy and of Cmin and AUC0-24 for safety of vancomycin. Is peak concentration needed in therapeutic drug monitoring of vancomycin?</t>
+  </si>
+  <si>
+    <t>Is peak concentration needed in therapeutic drug monitoring of vancomycin?</t>
+  </si>
+  <si>
+    <t>No, trough concentration is sufficient for therapeutic drug monitoring of vancomycin. The peak concentration of vancomycin is difficult to predict and not clinically relevant. The trough concentration is the most reliable predictor of efficacy and safety of vancomycin.</t>
+  </si>
+  <si>
+    <t>Given the variability in distribution, achieving therapeutic levels may be more relevant than targeting a specific peak concentration. However, higher loading doses can help ensure adequate exposure during the first days of treatment.</t>
+  </si>
+  <si>
+    <t>This investigation assesses the effect of platelet-rich plasma (PRP) gel on postoperative pain, swelling, and trismus as well as healing and bone regeneration potential on mandibular third molar extraction sockets. A prospective randomized comparative clinical study was undertaken over a 2-year period. Patients requiring surgical extraction of a single impacted third molar and who fell within the inclusion criteria and indicated willingness to return for recall visits were recruited. The predictor variable was application of PRP gel to the socket of the third molar in the test group, whereas the control group had no PRP. The outcome variables were pain, swelling, and maximum mouth opening, which were measured using a 10-point visual analog scale, tape, and millimeter caliper, respectively. Socket healing was assessed radiographically by allocating scores for lamina dura, overall density, and trabecular pattern. Quantitative data were presented as mean. Mann-Whitney test was used to compare means between groups for continuous variables, whereas Fischer exact test was used for categorical variables. Statistical significance was inferred at P&lt;.05. Sixty patients aged 19 to 35 years (mean: 24.7 ± 3.6 years) were divided into both test and control groups of 30 patients each. The mean postoperative pain score (visual analog scale) was lower for the PRP group at all time points and this was statistically significant (P&lt;.05). Although the figures for swelling and interincisal mouth opening were lower in the test group, this difference was not statistically significant. Similarly, the scores for lamina dura, trabecular pattern, and bone density were better among patients in the PRP group. This difference was also not statistically significant. Can autologous platelet-rich plasma gel enhance healing after surgical extraction of mandibular third molars?</t>
+  </si>
+  <si>
+    <t>Can autologous platelet-rich plasma gel enhance healing after surgical extraction of mandibular third molars?</t>
+  </si>
+  <si>
+    <t>Evidence indicates Potential for Positive Outcomes but further Research Designs are Needed; from Clinical Perspectives, it seems Plausible to Consider its Use.</t>
+  </si>
+  <si>
+    <t>I am a medical student who is interested in learning about the effects of platelet-rich plasma gel on postoperative pain, swelling, and trismus as well as healing and bone regeneration potential on mandibular third molar extraction sockets.</t>
+  </si>
+  <si>
+    <t>The reduced use of sugars-containing (SC) liquid medicines has increased the use of other dose forms, potentially resulting in more widespread dental effects, including tooth wear. The aim of this study was to assess the erosive potential of 97 paediatric medicines in vitro. The study took the form of in vitro measurement of endogenous pH and titratable acidity (mmol). Endogenous pH was measured using a pH meter, followed by titration to pH 7.0 with 0.1-M NaOH. Overall, 55 (57%) formulations had an endogenous pH of&lt;5.5. The mean (+/- SD) endogenous pH and titratable acidity for 41 SC formulations were 5.26 +/- 1.30 and 0.139 +/- 0.133 mmol, respectively; for 56 sugars-free (SF) formulations, these figures were 5.73 +/- 1.53 and 0.413 +/- 1.50 mmol (P&gt;0.05). Compared with their SC bioequivalents, eight SF medicines showed no significant differences for pH or titratable acidity, while 15 higher-strength medicines showed lower pH (P = 0.035) and greater titratable acidity (P = 0.016) than their lower-strength equivalents. Chewable and dispersible tablets (P&lt;0.001), gastrointestinal medicines (P = 0.002) and antibiotics (P = 0.007) were significant predictors of higher pH. In contrast, effervescent tablets (P&lt;0.001), and nutrition and blood preparations (P = 0.021) were significant predictors of higher titratable acidity. Are sugars-free medicines more erosive than sugars-containing medicines?</t>
+  </si>
+  <si>
+    <t>Are sugars-free medicines more erosive than sugars-containing medicines?</t>
+  </si>
+  <si>
+    <t>The reduced use of sugars-containing (SC) liquid medicines has increased the use of other dose forms, potentially resulting in more widespread dental effects, including tooth wear. The aim of this study was to assess the erosive potential of 97 paediatric medicines in vitro. The study took the form of in vitro measurement of endogenous pH and titratable acidity (mmol). Endogenous pH was measured using a pH meter, followed by titration to pH 7.0 with 0.1-M NaOH. Overall, 55 (57%) formulations had an endogenous pH of&lt;5.5. The mean (+/- SD) endogenous pH and titratable acidity for 41 SC formulations were 5.26 +/- 1.30 and 0.139 +/- 0.133 mmol, respectively; for 56 sugars-free (SF) formulations, these figures were 5.73 +/- 1.53 and 0.413 +/- 1.50 mmol</t>
+  </si>
+  <si>
+    <t>Although sugar coating may improve palatability, it can also increase the risk of enamel damage due to lower pH values. However, other factors like the type of vehicle and the frequency of use are often more critical for the risk of erosion.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -913,6 +1249,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -929,12 +1269,24 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1146,6 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3538,146 +3891,1535 @@
       </c>
     </row>
     <row r="409">
-      <c r="A409" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C409" s="1" t="s">
+      <c r="A409" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B409" s="3"/>
+      <c r="C409" s="4" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="410">
-      <c r="A410" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C410" s="1" t="s">
+      <c r="A410" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B410" s="3"/>
+      <c r="C410" s="4" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="411">
-      <c r="A411" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B411" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C411" s="1" t="s">
+      <c r="A411" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B411" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C411" s="4" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="412">
-      <c r="A412" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C412" s="1" t="s">
+      <c r="A412" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B412" s="3"/>
+      <c r="C412" s="4" t="s">
         <v>282</v>
       </c>
     </row>
+    <row r="413">
+      <c r="A413" s="3"/>
+      <c r="B413" s="3"/>
+      <c r="C413" s="3"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="3"/>
+      <c r="B414" s="3"/>
+      <c r="C414" s="3"/>
+    </row>
     <row r="415">
-      <c r="A415" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C415" s="1" t="s">
+      <c r="A415" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B415" s="3"/>
+      <c r="C415" s="4" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="416">
-      <c r="A416" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C416" s="1" t="s">
+      <c r="A416" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B416" s="3"/>
+      <c r="C416" s="4" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="417">
-      <c r="A417" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B417" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C417" s="1" t="s">
+      <c r="A417" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B417" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C417" s="4" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="418">
-      <c r="A418" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C418" s="1" t="s">
+      <c r="A418" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B418" s="3"/>
+      <c r="C418" s="4" t="s">
         <v>286</v>
       </c>
     </row>
+    <row r="419">
+      <c r="A419" s="3"/>
+      <c r="B419" s="3"/>
+      <c r="C419" s="3"/>
+    </row>
+    <row r="420">
+      <c r="A420" s="3"/>
+      <c r="B420" s="3"/>
+      <c r="C420" s="3"/>
+    </row>
     <row r="421">
-      <c r="A421" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C421" s="1" t="s">
+      <c r="A421" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B421" s="3"/>
+      <c r="C421" s="4" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="422">
-      <c r="A422" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C422" s="1" t="s">
+      <c r="A422" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B422" s="3"/>
+      <c r="C422" s="4" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="423">
-      <c r="A423" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C423" s="1" t="s">
+      <c r="A423" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B423" s="3"/>
+      <c r="C423" s="4" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="424">
-      <c r="A424" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B424" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C424" s="1" t="s">
+      <c r="A424" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B424" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C424" s="4" t="s">
         <v>290</v>
       </c>
     </row>
+    <row r="425">
+      <c r="A425" s="3"/>
+      <c r="B425" s="3"/>
+      <c r="C425" s="3"/>
+    </row>
+    <row r="426">
+      <c r="A426" s="3"/>
+      <c r="B426" s="3"/>
+      <c r="C426" s="3"/>
+    </row>
     <row r="427">
-      <c r="A427" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C427" s="1" t="s">
+      <c r="A427" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B427" s="3"/>
+      <c r="C427" s="4" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="428">
-      <c r="A428" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C428" s="1" t="s">
+      <c r="A428" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B428" s="3"/>
+      <c r="C428" s="4" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="429">
-      <c r="A429" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B429" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C429" s="1" t="s">
+      <c r="A429" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B429" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C429" s="4" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="430">
-      <c r="A430" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C430" s="1" t="s">
+      <c r="A430" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B430" s="3"/>
+      <c r="C430" s="4" t="s">
         <v>294</v>
       </c>
     </row>
+    <row r="431">
+      <c r="A431" s="3"/>
+      <c r="B431" s="3"/>
+      <c r="C431" s="3"/>
+    </row>
+    <row r="432">
+      <c r="A432" s="3"/>
+      <c r="B432" s="3"/>
+      <c r="C432" s="3"/>
+    </row>
+    <row r="433">
+      <c r="A433" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B433" s="3"/>
+      <c r="C433" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B434" s="3"/>
+      <c r="C434" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B435" s="3"/>
+      <c r="C435" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B436" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C436" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="3"/>
+      <c r="B437" s="3"/>
+      <c r="C437" s="3"/>
+    </row>
+    <row r="438">
+      <c r="A438" s="3"/>
+      <c r="B438" s="3"/>
+      <c r="C438" s="3"/>
+    </row>
+    <row r="439">
+      <c r="A439" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B439" s="3"/>
+      <c r="C439" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B440" s="3"/>
+      <c r="C440" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B441" s="3"/>
+      <c r="C441" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B442" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C442" s="5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="3"/>
+      <c r="B443" s="3"/>
+      <c r="C443" s="3"/>
+    </row>
+    <row r="444">
+      <c r="A444" s="3"/>
+      <c r="B444" s="3"/>
+      <c r="C444" s="3"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B445" s="3"/>
+      <c r="C445" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B446" s="3"/>
+      <c r="C446" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B447" s="3"/>
+      <c r="C447" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B448" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C448" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="3"/>
+      <c r="B449" s="3"/>
+      <c r="C449" s="3"/>
+    </row>
+    <row r="450">
+      <c r="A450" s="3"/>
+      <c r="B450" s="3"/>
+      <c r="C450" s="3"/>
+    </row>
+    <row r="451">
+      <c r="A451" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B451" s="3"/>
+      <c r="C451" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B452" s="3"/>
+      <c r="C452" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B453" s="3"/>
+      <c r="C453" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B454" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C454" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="3"/>
+      <c r="B455" s="3"/>
+      <c r="C455" s="3"/>
+    </row>
+    <row r="456">
+      <c r="A456" s="3"/>
+      <c r="B456" s="3"/>
+      <c r="C456" s="3"/>
+    </row>
+    <row r="457">
+      <c r="A457" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B457" s="3"/>
+      <c r="C457" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B458" s="3"/>
+      <c r="C458" s="5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B459" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C459" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B460" s="3"/>
+      <c r="C460" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="3"/>
+      <c r="B461" s="3"/>
+      <c r="C461" s="3"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="3"/>
+      <c r="B462" s="3"/>
+      <c r="C462" s="3"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B463" s="3"/>
+      <c r="C463" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B464" s="3"/>
+      <c r="C464" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B465" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C465" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B466" s="3"/>
+      <c r="C466" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="3"/>
+      <c r="B467" s="3"/>
+      <c r="C467" s="3"/>
+    </row>
+    <row r="468">
+      <c r="A468" s="3"/>
+      <c r="B468" s="3"/>
+      <c r="C468" s="3"/>
+    </row>
+    <row r="469">
+      <c r="A469" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B469" s="3"/>
+      <c r="C469" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B470" s="3"/>
+      <c r="C470" s="5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B471" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C471" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B472" s="3"/>
+      <c r="C472" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="3"/>
+      <c r="B473" s="3"/>
+      <c r="C473" s="3"/>
+    </row>
+    <row r="474">
+      <c r="A474" s="3"/>
+      <c r="B474" s="3"/>
+      <c r="C474" s="3"/>
+    </row>
+    <row r="475">
+      <c r="A475" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B475" s="3"/>
+      <c r="C475" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B476" s="3"/>
+      <c r="C476" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B477" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C477" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B478" s="3"/>
+      <c r="C478" s="5" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="3"/>
+      <c r="B479" s="3"/>
+      <c r="C479" s="3"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="3"/>
+      <c r="B480" s="3"/>
+      <c r="C480" s="3"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B481" s="3"/>
+      <c r="C481" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B482" s="3"/>
+      <c r="C482" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B483" s="3"/>
+      <c r="C483" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B484" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C484" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="3"/>
+      <c r="B485" s="3"/>
+      <c r="C485" s="3"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="3"/>
+      <c r="B486" s="3"/>
+      <c r="C486" s="3"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B487" s="3"/>
+      <c r="C487" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B488" s="3"/>
+      <c r="C488" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B489" s="3"/>
+      <c r="C489" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B490" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C490" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="3"/>
+      <c r="B491" s="3"/>
+      <c r="C491" s="3"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="3"/>
+      <c r="B492" s="3"/>
+      <c r="C492" s="3"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B493" s="3"/>
+      <c r="C493" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B494" s="3"/>
+      <c r="C494" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B495" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C495" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B496" s="3"/>
+      <c r="C496" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="3"/>
+      <c r="B497" s="3"/>
+      <c r="C497" s="3"/>
+    </row>
+    <row r="498">
+      <c r="A498" s="3"/>
+      <c r="B498" s="3"/>
+      <c r="C498" s="3"/>
+    </row>
+    <row r="499">
+      <c r="A499" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B499" s="3"/>
+      <c r="C499" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B500" s="3"/>
+      <c r="C500" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B501" s="3"/>
+      <c r="C501" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B502" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C502" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="3"/>
+      <c r="B503" s="3"/>
+      <c r="C503" s="3"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="3"/>
+      <c r="B504" s="3"/>
+      <c r="C504" s="3"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B505" s="3"/>
+      <c r="C505" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B506" s="3"/>
+      <c r="C506" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B507" s="3"/>
+      <c r="C507" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B508" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C508" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="3"/>
+      <c r="B509" s="3"/>
+      <c r="C509" s="3"/>
+    </row>
+    <row r="510">
+      <c r="A510" s="3"/>
+      <c r="B510" s="3"/>
+      <c r="C510" s="3"/>
+    </row>
+    <row r="511">
+      <c r="A511" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B511" s="3"/>
+      <c r="C511" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B512" s="3"/>
+      <c r="C512" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B513" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C513" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B514" s="3"/>
+      <c r="C514" s="5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="3"/>
+      <c r="B515" s="3"/>
+      <c r="C515" s="3"/>
+    </row>
+    <row r="516">
+      <c r="A516" s="3"/>
+      <c r="B516" s="3"/>
+      <c r="C516" s="3"/>
+    </row>
+    <row r="517">
+      <c r="A517" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B517" s="3"/>
+      <c r="C517" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B518" s="3"/>
+      <c r="C518" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B519" s="3"/>
+      <c r="C519" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B520" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C520" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="3"/>
+      <c r="B521" s="3"/>
+      <c r="C521" s="3"/>
+    </row>
+    <row r="522">
+      <c r="A522" s="3"/>
+      <c r="B522" s="3"/>
+      <c r="C522" s="3"/>
+    </row>
+    <row r="523">
+      <c r="A523" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B523" s="3"/>
+      <c r="C523" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B524" s="3"/>
+      <c r="C524" s="5" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B525" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C525" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B526" s="3"/>
+      <c r="C526" s="5" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="3"/>
+      <c r="B527" s="3"/>
+      <c r="C527" s="3"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="3"/>
+      <c r="B528" s="3"/>
+      <c r="C528" s="3"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B529" s="3"/>
+      <c r="C529" s="5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B530" s="3"/>
+      <c r="C530" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B531" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C531" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B532" s="3"/>
+      <c r="C532" s="5" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="3"/>
+      <c r="B533" s="3"/>
+      <c r="C533" s="3"/>
+    </row>
+    <row r="534">
+      <c r="A534" s="3"/>
+      <c r="B534" s="3"/>
+      <c r="C534" s="3"/>
+    </row>
+    <row r="535">
+      <c r="A535" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B535" s="3"/>
+      <c r="C535" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B536" s="3"/>
+      <c r="C536" s="5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B537" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C537" s="5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B538" s="3"/>
+      <c r="C538" s="5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="3"/>
+      <c r="B539" s="3"/>
+      <c r="C539" s="3"/>
+    </row>
+    <row r="540">
+      <c r="A540" s="3"/>
+      <c r="B540" s="3"/>
+      <c r="C540" s="3"/>
+    </row>
+    <row r="541">
+      <c r="A541" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B541" s="3"/>
+      <c r="C541" s="5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B542" s="3"/>
+      <c r="C542" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B543" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C543" s="5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B544" s="3"/>
+      <c r="C544" s="5" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="3"/>
+      <c r="B545" s="3"/>
+      <c r="C545" s="3"/>
+    </row>
+    <row r="546">
+      <c r="A546" s="3"/>
+      <c r="B546" s="3"/>
+      <c r="C546" s="3"/>
+    </row>
+    <row r="547">
+      <c r="A547" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B547" s="3"/>
+      <c r="C547" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B548" s="3"/>
+      <c r="C548" s="5" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B549" s="3"/>
+      <c r="C549" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B550" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C550" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="3"/>
+      <c r="B551" s="3"/>
+      <c r="C551" s="3"/>
+    </row>
+    <row r="552">
+      <c r="A552" s="3"/>
+      <c r="B552" s="3"/>
+      <c r="C552" s="3"/>
+    </row>
+    <row r="553">
+      <c r="A553" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B553" s="3"/>
+      <c r="C553" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B554" s="3"/>
+      <c r="C554" s="5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B555" s="3"/>
+      <c r="C555" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B556" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C556" s="5" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="3"/>
+      <c r="B557" s="3"/>
+      <c r="C557" s="3"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="3"/>
+      <c r="B558" s="3"/>
+      <c r="C558" s="3"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B559" s="3"/>
+      <c r="C559" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B560" s="3"/>
+      <c r="C560" s="5" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B561" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C561" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B562" s="3"/>
+      <c r="C562" s="5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="3"/>
+      <c r="B563" s="3"/>
+      <c r="C563" s="3"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="3"/>
+      <c r="B564" s="3"/>
+      <c r="C564" s="3"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B565" s="3"/>
+      <c r="C565" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B566" s="3"/>
+      <c r="C566" s="5" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B567" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C567" s="5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B568" s="3"/>
+      <c r="C568" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="3"/>
+      <c r="B569" s="3"/>
+      <c r="C569" s="3"/>
+    </row>
+    <row r="570">
+      <c r="A570" s="3"/>
+      <c r="B570" s="3"/>
+      <c r="C570" s="3"/>
+    </row>
+    <row r="571">
+      <c r="A571" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B571" s="3"/>
+      <c r="C571" s="5" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B572" s="3"/>
+      <c r="C572" s="5" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B573" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C573" s="5" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B574" s="3"/>
+      <c r="C574" s="5" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="3"/>
+      <c r="B575" s="3"/>
+      <c r="C575" s="3"/>
+    </row>
+    <row r="576">
+      <c r="A576" s="3"/>
+      <c r="B576" s="3"/>
+      <c r="C576" s="3"/>
+    </row>
+    <row r="577">
+      <c r="A577" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B577" s="3"/>
+      <c r="C577" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B578" s="3"/>
+      <c r="C578" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B579" s="3"/>
+      <c r="C579" s="5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B580" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C580" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="3"/>
+      <c r="B581" s="3"/>
+      <c r="C581" s="3"/>
+    </row>
+    <row r="582">
+      <c r="A582" s="3"/>
+      <c r="B582" s="3"/>
+      <c r="C582" s="3"/>
+    </row>
+    <row r="583">
+      <c r="A583" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B583" s="3"/>
+      <c r="C583" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B584" s="3"/>
+      <c r="C584" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B585" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C585" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B586" s="3"/>
+      <c r="C586" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="3"/>
+      <c r="B587" s="3"/>
+      <c r="C587" s="3"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="3"/>
+      <c r="B588" s="3"/>
+      <c r="C588" s="3"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B589" s="3"/>
+      <c r="C589" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B590" s="3"/>
+      <c r="C590" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B591" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C591" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B592" s="3"/>
+      <c r="C592" s="5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" s="3"/>
+      <c r="B593" s="3"/>
+      <c r="C593" s="3"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="3"/>
+      <c r="B594" s="3"/>
+      <c r="C594" s="3"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B595" s="3"/>
+      <c r="C595" s="5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B596" s="3"/>
+      <c r="C596" s="5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B597" s="3"/>
+      <c r="C597" s="5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B598" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C598" s="5" t="s">
+        <v>406</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>